<commit_message>
added table for product list
</commit_message>
<xml_diff>
--- a/ASIN-1.xlsx
+++ b/ASIN-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\web-scapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F732ACA5-D1AF-414B-9339-F12DA6CFB4B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0965792E-55C8-4EEC-9EFE-C9E682ED2349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2512" yWindow="2512" windowWidth="16201" windowHeight="9308" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,9 +28,6 @@
     <t>B0D18MZ48T</t>
   </si>
   <si>
-    <t>B0CD8YLKN2</t>
-  </si>
-  <si>
     <t>B073R5692B</t>
   </si>
   <si>
@@ -50,6 +47,9 @@
   </si>
   <si>
     <t>B093WZZLL7</t>
+  </si>
+  <si>
+    <t>B0B15QM5LL</t>
   </si>
 </sst>
 </file>
@@ -407,7 +407,7 @@
   <dimension ref="A1:A100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
@@ -423,7 +423,7 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14.25">
@@ -433,37 +433,37 @@
     </row>
     <row r="4" spans="1:1" ht="14.25">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="14.25">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="14.25">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="14.25">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="14.25">
       <c r="A8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="14.25">
       <c r="A9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="14.25">
       <c r="A10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="14.25">

</xml_diff>